<commit_message>
Added Ticket.feature and DD scenarios
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/TestData.xlsx
+++ b/src/test/resources/Data/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunilsonwane\AutomationTestHub\Maven_test\BDD\src\test\resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunilsonwane\AutomationTestHub\Maven_test\CucumberFrameworkAug2024\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE36D08-1317-48B3-936D-3619511678A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB39497-8DDE-45B2-B134-B51309044A36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11796" yWindow="0" windowWidth="10272" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
   <si>
     <t>UserId</t>
   </si>
@@ -109,6 +109,18 @@
   </si>
   <si>
     <t>TC_06_Create_Potential</t>
+  </si>
+  <si>
+    <t>TC_07_Check Priority DD in New Ticket page</t>
+  </si>
+  <si>
+    <t>Aqua</t>
+  </si>
+  <si>
+    <t>TC_08_Check Severity DD in New Ticket page</t>
+  </si>
+  <si>
+    <t>TC_09_Check category DD in New Ticket page</t>
   </si>
 </sst>
 </file>
@@ -468,15 +480,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="37.88671875" customWidth="1"/>
+    <col min="1" max="1" width="48.33203125" customWidth="1"/>
     <col min="8" max="8" width="16.44140625" customWidth="1"/>
     <col min="9" max="9" width="14.33203125" customWidth="1"/>
   </cols>
@@ -632,16 +644,62 @@
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="A8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Changes to implement Ticket_Featur including handling alert and DD
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/TestData.xlsx
+++ b/src/test/resources/Data/TestData.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunilsonwane\AutomationTestHub\Maven_test\CucumberFrameworkAug2024\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB39497-8DDE-45B2-B134-B51309044A36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{278E3CBF-7235-44B3-85BF-EED71F4D2528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
   <si>
     <t>UserId</t>
   </si>
@@ -111,16 +122,43 @@
     <t>TC_06_Create_Potential</t>
   </si>
   <si>
-    <t>TC_07_Check Priority DD in New Ticket page</t>
-  </si>
-  <si>
     <t>Aqua</t>
   </si>
   <si>
-    <t>TC_08_Check Severity DD in New Ticket page</t>
-  </si>
-  <si>
     <t>TC_09_Check category DD in New Ticket page</t>
+  </si>
+  <si>
+    <t>TC_07_Check Priority, Severity and Category DD in New Ticket page</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Severity</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">,  , </t>
+  </si>
+  <si>
+    <t>Other Problem</t>
+  </si>
+  <si>
+    <t>Test_User</t>
+  </si>
+  <si>
+    <t>TC_08_Check Alert for Mandatory Fields and save mandatory fields in New Ticket page</t>
+  </si>
+  <si>
+    <t>TC_10_Create_Lead_Data from Page Factory</t>
   </si>
 </sst>
 </file>
@@ -163,7 +201,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -186,11 +224,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -200,6 +249,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -491,9 +542,10 @@
     <col min="1" max="1" width="48.33203125" customWidth="1"/>
     <col min="8" max="8" width="16.44140625" customWidth="1"/>
     <col min="9" max="9" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -521,8 +573,17 @@
       <c r="I1" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -538,8 +599,11 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -555,8 +619,11 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -577,8 +644,11 @@
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
@@ -598,8 +668,11 @@
         <v>18</v>
       </c>
       <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -621,8 +694,11 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
@@ -642,29 +718,40 @@
       <c r="I7" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="2" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>8</v>
@@ -675,15 +762,20 @@
       <c r="D9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="E9" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="4" t="s">
-        <v>31</v>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>8</v>
@@ -699,6 +791,36 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+    </row>
+    <row r="17" spans="8:8">
+      <c r="H17" s="4" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changes to integrate - Potential page - include Handle windows
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/TestData.xlsx
+++ b/src/test/resources/Data/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunilsonwane\AutomationTestHub\Maven_test\CucumberFrameworkAug2024\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{278E3CBF-7235-44B3-85BF-EED71F4D2528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE95B45D-EF6B-4C39-B36B-8637B1FBCC5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
   <si>
     <t>UserId</t>
   </si>
@@ -144,9 +144,6 @@
   </si>
   <si>
     <t>Feature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">,  , </t>
   </si>
   <si>
     <t>Other Problem</t>
@@ -534,7 +531,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -746,12 +743,12 @@
         <v>35</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>8</v>
@@ -763,7 +760,7 @@
         <v>16</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -797,7 +794,7 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>8</v>
@@ -818,9 +815,7 @@
       <c r="L11" s="3"/>
     </row>
     <row r="17" spans="8:8">
-      <c r="H17" s="4" t="s">
-        <v>36</v>
-      </c>
+      <c r="H17" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
chenages around web table and all
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/TestData.xlsx
+++ b/src/test/resources/Data/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunilsonwane\AutomationTestHub\Maven_test\CucumberFrameworkAug2024\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE95B45D-EF6B-4C39-B36B-8637B1FBCC5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D67A733-791C-4DF9-8884-358A0B4443F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="44">
   <si>
     <t>UserId</t>
   </si>
@@ -156,13 +156,25 @@
   </si>
   <si>
     <t>TC_10_Create_Lead_Data from Page Factory</t>
+  </si>
+  <si>
+    <t>TC_11_Validate Login Page Links</t>
+  </si>
+  <si>
+    <t>Senior QA Lead</t>
+  </si>
+  <si>
+    <t>QA_@123</t>
+  </si>
+  <si>
+    <t>TC_12_Validate New Vendor Page</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,6 +194,14 @@
       <color rgb="FF080808"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -233,10 +253,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -248,8 +269,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -531,12 +554,14 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="48.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.21875" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" customWidth="1"/>
     <col min="8" max="8" width="16.44140625" customWidth="1"/>
     <col min="9" max="9" width="14.33203125" customWidth="1"/>
     <col min="12" max="12" width="12.44140625" customWidth="1"/>
@@ -814,11 +839,67 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+    </row>
     <row r="17" spans="8:8">
       <c r="H17" s="4"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F12" r:id="rId1" xr:uid="{344F5BE8-7034-4338-8EC8-22EA44B5FE79}"/>
+    <hyperlink ref="F13" r:id="rId2" xr:uid="{5FCAB708-110B-4BB2-A3FD-7301EACD1D4D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>